<commit_message>
updated bom with purchase costs.
</commit_message>
<xml_diff>
--- a/T-06 BOM.xlsx
+++ b/T-06 BOM.xlsx
@@ -5,21 +5,23 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tyler\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\khensu\Home05\seitzt\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="12570"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="T06-SCHEMATIC-INTERCOM-REVA" sheetId="1" r:id="rId1"/>
+    <sheet name="Consolidated, NO DNIs" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
+    <sheet name="T06-SCHEMATIC-INTERCOM-REVA" sheetId="1" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="215">
   <si>
     <t>T-06 Intercom  Revised: Tuesday, November 29, 2016</t>
   </si>
@@ -643,12 +645,36 @@
   </si>
   <si>
     <t>1.) T-06 INTERCOM          Revision: A</t>
+  </si>
+  <si>
+    <t>0603</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>Line Cost*</t>
+  </si>
+  <si>
+    <t>*Line cost uses unit build quantities of less than 10.</t>
+  </si>
+  <si>
+    <t>PCB</t>
+  </si>
+  <si>
+    <t>TOTAL PER UNIT:</t>
+  </si>
+  <si>
+    <t>PARTS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+  </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1150,7 +1176,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1159,6 +1185,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1482,10 +1517,1734 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I79"/>
+  <sheetViews>
+    <sheetView topLeftCell="E6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A8" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="32.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="27.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.28515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.140625" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" s="3"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>1</v>
+      </c>
+      <c r="B8" s="2">
+        <v>13</v>
+      </c>
+      <c r="C8" s="6">
+        <v>1.3</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" s="3"/>
+      <c r="C9" s="6">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>2</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1</v>
+      </c>
+      <c r="C10" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H10" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <v>3</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1</v>
+      </c>
+      <c r="C11" s="6">
+        <v>0.11</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>4</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1</v>
+      </c>
+      <c r="C12" s="6">
+        <v>0.15</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>5</v>
+      </c>
+      <c r="B13" s="2">
+        <v>3</v>
+      </c>
+      <c r="C13" s="6">
+        <v>1.29</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="I13" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <v>6</v>
+      </c>
+      <c r="B14" s="2">
+        <v>3</v>
+      </c>
+      <c r="C14" s="6">
+        <v>0.81</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
+        <v>7</v>
+      </c>
+      <c r="B15" s="2">
+        <v>6</v>
+      </c>
+      <c r="C15" s="6">
+        <v>1.62</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <v>8</v>
+      </c>
+      <c r="B16" s="2">
+        <v>1</v>
+      </c>
+      <c r="C16" s="6">
+        <v>0.13</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="F16" s="4">
+        <v>1206</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="I16" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
+        <v>9</v>
+      </c>
+      <c r="B17" s="2">
+        <v>1</v>
+      </c>
+      <c r="C17" s="6">
+        <v>1.38</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
+        <v>10</v>
+      </c>
+      <c r="B18" s="2">
+        <v>1</v>
+      </c>
+      <c r="C18" s="6">
+        <v>0.28166666666666668</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
+        <v>11</v>
+      </c>
+      <c r="B19" s="2">
+        <v>2</v>
+      </c>
+      <c r="C19" s="6">
+        <v>2.1</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="3">
+        <v>12</v>
+      </c>
+      <c r="B20" s="2">
+        <v>1</v>
+      </c>
+      <c r="C20" s="6">
+        <v>0.39</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="F20" s="4">
+        <v>1210</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
+        <v>13</v>
+      </c>
+      <c r="B21" s="2">
+        <v>8</v>
+      </c>
+      <c r="C21" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="3"/>
+      <c r="C22" s="6">
+        <v>0</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="3">
+        <v>14</v>
+      </c>
+      <c r="B23" s="2">
+        <v>7</v>
+      </c>
+      <c r="C23" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="3"/>
+      <c r="C24" s="6">
+        <v>0</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="3">
+        <v>15</v>
+      </c>
+      <c r="B25" s="2">
+        <v>1</v>
+      </c>
+      <c r="C25" s="6">
+        <v>1.05</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A26" s="3">
+        <v>16</v>
+      </c>
+      <c r="B26" s="2">
+        <v>1</v>
+      </c>
+      <c r="C26" s="6">
+        <v>3.53</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A27" s="3">
+        <v>17</v>
+      </c>
+      <c r="B27" s="2">
+        <v>5</v>
+      </c>
+      <c r="C27" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I27" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="3">
+        <v>18</v>
+      </c>
+      <c r="B28" s="2">
+        <v>3</v>
+      </c>
+      <c r="C28" s="6">
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="E28" s="4">
+        <v>0</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="H28" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" s="3">
+        <v>19</v>
+      </c>
+      <c r="B29" s="2">
+        <v>2</v>
+      </c>
+      <c r="C29" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="E29" s="4">
+        <v>33</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" s="3">
+        <v>20</v>
+      </c>
+      <c r="B30" s="2">
+        <v>8</v>
+      </c>
+      <c r="C30" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="H30" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I30" s="4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="3"/>
+      <c r="C31" s="6">
+        <v>0</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="3">
+        <v>21</v>
+      </c>
+      <c r="B32" s="2">
+        <v>2</v>
+      </c>
+      <c r="C32" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="H32" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I32" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" s="3">
+        <v>22</v>
+      </c>
+      <c r="B33" s="2">
+        <v>4</v>
+      </c>
+      <c r="C33" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="E33" s="4">
+        <v>100</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="H33" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="I33" s="4" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="3">
+        <v>23</v>
+      </c>
+      <c r="B34" s="2">
+        <v>7</v>
+      </c>
+      <c r="C34" s="6">
+        <v>3.01</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" s="3">
+        <v>24</v>
+      </c>
+      <c r="B35" s="2">
+        <v>1</v>
+      </c>
+      <c r="C35" s="6">
+        <v>0.88</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="H35" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="I35" s="4" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" s="3">
+        <v>25</v>
+      </c>
+      <c r="B36" s="2">
+        <v>1</v>
+      </c>
+      <c r="C36" s="6">
+        <v>2.29</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="H36" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="I36" s="4" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A37" s="3">
+        <v>26</v>
+      </c>
+      <c r="B37" s="2">
+        <v>1</v>
+      </c>
+      <c r="C37" s="6">
+        <v>4.51</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="H37" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="I37" s="4" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A38" s="3">
+        <v>27</v>
+      </c>
+      <c r="B38" s="2">
+        <v>1</v>
+      </c>
+      <c r="C38" s="6">
+        <v>0.46</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="F38" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="H38" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="I38" s="4" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A39" s="3">
+        <v>28</v>
+      </c>
+      <c r="C39" s="6">
+        <v>0</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="F39" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="H39" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="I39" s="4" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A40" s="3">
+        <v>29</v>
+      </c>
+      <c r="B40" s="2">
+        <v>1</v>
+      </c>
+      <c r="C40" s="6">
+        <v>0.43</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="F40" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="H40" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="I40" s="4" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A41" s="3">
+        <v>30</v>
+      </c>
+      <c r="B41" s="2">
+        <v>1</v>
+      </c>
+      <c r="C41" s="6">
+        <v>18</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C43" s="6">
+        <f>SUM(C8:C40)</f>
+        <v>29.221666666666664</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C44" s="6">
+        <f>C41</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C46" s="6">
+        <f>SUM(C8:C41)</f>
+        <v>47.221666666666664</v>
+      </c>
+      <c r="D46" s="6"/>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D47" s="6"/>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="D48" s="6"/>
+    </row>
+    <row r="49" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D49" s="6"/>
+    </row>
+    <row r="50" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D50" s="6"/>
+    </row>
+    <row r="51" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D51" s="6"/>
+    </row>
+    <row r="52" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D52" s="6"/>
+    </row>
+    <row r="53" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D53" s="6"/>
+    </row>
+    <row r="54" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D54" s="6"/>
+    </row>
+    <row r="55" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D55" s="6"/>
+    </row>
+    <row r="56" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D56" s="6"/>
+    </row>
+    <row r="57" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D57" s="6"/>
+    </row>
+    <row r="58" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D58" s="6"/>
+    </row>
+    <row r="59" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D59" s="6"/>
+    </row>
+    <row r="60" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D60" s="6"/>
+    </row>
+    <row r="61" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D61" s="6"/>
+    </row>
+    <row r="62" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D62" s="6"/>
+    </row>
+    <row r="63" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D63" s="6"/>
+    </row>
+    <row r="64" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D64" s="6"/>
+    </row>
+    <row r="65" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D65" s="6"/>
+    </row>
+    <row r="66" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D66" s="6"/>
+    </row>
+    <row r="67" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D67" s="6"/>
+    </row>
+    <row r="68" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D68" s="6"/>
+    </row>
+    <row r="69" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D69" s="6"/>
+    </row>
+    <row r="70" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D70" s="6"/>
+    </row>
+    <row r="71" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D71" s="6"/>
+    </row>
+    <row r="72" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D72" s="6"/>
+    </row>
+    <row r="73" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D73" s="6"/>
+    </row>
+    <row r="74" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D74" s="6"/>
+    </row>
+    <row r="75" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D75" s="6"/>
+    </row>
+    <row r="76" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D76" s="6"/>
+    </row>
+    <row r="77" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D77" s="6"/>
+    </row>
+    <row r="78" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D78" s="6"/>
+    </row>
+    <row r="79" spans="4:4" x14ac:dyDescent="0.3">
+      <c r="D79" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="21.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.42578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="3"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="3">
+        <v>1</v>
+      </c>
+      <c r="B8" s="2">
+        <v>13</v>
+      </c>
+      <c r="C8" s="6">
+        <v>1.3</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9" s="3"/>
+      <c r="C9" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="3">
+        <v>2</v>
+      </c>
+      <c r="B10" s="2">
+        <v>1</v>
+      </c>
+      <c r="C10" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11" s="3">
+        <v>3</v>
+      </c>
+      <c r="B11" s="2">
+        <v>1</v>
+      </c>
+      <c r="C11" s="6">
+        <v>0.11</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="3">
+        <v>4</v>
+      </c>
+      <c r="B12" s="2">
+        <v>1</v>
+      </c>
+      <c r="C12" s="6">
+        <v>0.15</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="3">
+        <v>5</v>
+      </c>
+      <c r="B13" s="2">
+        <v>3</v>
+      </c>
+      <c r="C13" s="6">
+        <v>1.29</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="3">
+        <v>6</v>
+      </c>
+      <c r="B14" s="2">
+        <v>3</v>
+      </c>
+      <c r="C14" s="6">
+        <v>0.81</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="3">
+        <v>7</v>
+      </c>
+      <c r="B15" s="2">
+        <v>6</v>
+      </c>
+      <c r="C15" s="6">
+        <v>1.62</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="3">
+        <v>8</v>
+      </c>
+      <c r="B16" s="2">
+        <v>1</v>
+      </c>
+      <c r="C16" s="6">
+        <v>0.13</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E16" s="4">
+        <v>1206</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="3">
+        <v>9</v>
+      </c>
+      <c r="B17" s="2">
+        <v>1</v>
+      </c>
+      <c r="C17" s="6">
+        <v>1.38</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="3">
+        <v>10</v>
+      </c>
+      <c r="B18" s="2">
+        <v>1</v>
+      </c>
+      <c r="C18" s="6">
+        <v>0.28166666666666668</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="3">
+        <v>11</v>
+      </c>
+      <c r="B19" s="2">
+        <v>2</v>
+      </c>
+      <c r="C19" s="6">
+        <v>2.1</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="3">
+        <v>12</v>
+      </c>
+      <c r="B20" s="2">
+        <v>1</v>
+      </c>
+      <c r="C20" s="6">
+        <v>0.39</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="E20" s="4">
+        <v>1210</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="3">
+        <v>13</v>
+      </c>
+      <c r="B21" s="2">
+        <v>8</v>
+      </c>
+      <c r="C21" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="3"/>
+      <c r="C22" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="3">
+        <v>14</v>
+      </c>
+      <c r="B23" s="2">
+        <v>7</v>
+      </c>
+      <c r="C23" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="3"/>
+      <c r="C24" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="3">
+        <v>15</v>
+      </c>
+      <c r="B25" s="2">
+        <v>1</v>
+      </c>
+      <c r="C25" s="6">
+        <v>1.05</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="3">
+        <v>16</v>
+      </c>
+      <c r="B26" s="2">
+        <v>1</v>
+      </c>
+      <c r="C26" s="6">
+        <v>3.53</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="3">
+        <v>17</v>
+      </c>
+      <c r="B27" s="2">
+        <v>5</v>
+      </c>
+      <c r="C27" s="6">
+        <v>0.5</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="3">
+        <v>18</v>
+      </c>
+      <c r="B28" s="2">
+        <v>3</v>
+      </c>
+      <c r="C28" s="6">
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="D28" s="4">
+        <v>0</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="3">
+        <v>19</v>
+      </c>
+      <c r="B29" s="2">
+        <v>2</v>
+      </c>
+      <c r="C29" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="D29" s="4">
+        <v>33</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="3">
+        <v>20</v>
+      </c>
+      <c r="B30" s="2">
+        <v>8</v>
+      </c>
+      <c r="C30" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="3"/>
+      <c r="C31" s="6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="3">
+        <v>21</v>
+      </c>
+      <c r="B32" s="2">
+        <v>2</v>
+      </c>
+      <c r="C32" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A33" s="3">
+        <v>22</v>
+      </c>
+      <c r="B33" s="2">
+        <v>4</v>
+      </c>
+      <c r="C33" s="6">
+        <v>0.4</v>
+      </c>
+      <c r="D33" s="4">
+        <v>100</v>
+      </c>
+      <c r="E33" s="4" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A34" s="3">
+        <v>23</v>
+      </c>
+      <c r="B34" s="2">
+        <v>7</v>
+      </c>
+      <c r="C34" s="6">
+        <v>3.01</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A35" s="3">
+        <v>24</v>
+      </c>
+      <c r="B35" s="2">
+        <v>1</v>
+      </c>
+      <c r="C35" s="6">
+        <v>0.88</v>
+      </c>
+      <c r="D35" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="E35" s="4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A36" s="3">
+        <v>25</v>
+      </c>
+      <c r="B36" s="2">
+        <v>1</v>
+      </c>
+      <c r="C36" s="6">
+        <v>2.29</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A37" s="3">
+        <v>26</v>
+      </c>
+      <c r="B37" s="2">
+        <v>1</v>
+      </c>
+      <c r="C37" s="6">
+        <v>4.51</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A38" s="3">
+        <v>27</v>
+      </c>
+      <c r="B38" s="2">
+        <v>1</v>
+      </c>
+      <c r="C38" s="6">
+        <v>0.46</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A39" s="3">
+        <v>28</v>
+      </c>
+      <c r="C39" s="6">
+        <v>0</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="E39" s="4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A40" s="3">
+        <v>29</v>
+      </c>
+      <c r="B40" s="2">
+        <v>1</v>
+      </c>
+      <c r="C40" s="6">
+        <v>0.43</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="E40" s="4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A41" s="3">
+        <v>30</v>
+      </c>
+      <c r="B41" s="2">
+        <v>1</v>
+      </c>
+      <c r="C41" s="6">
+        <v>18</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A43" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C43" s="6">
+        <f>SUM(C8:C40)</f>
+        <v>29.221666666666664</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A44" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C44" s="6">
+        <f>C41</f>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A46" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="C46" s="6">
+        <f>SUM(C8:C41)</f>
+        <v>47.221666666666664</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>

</xml_diff>